<commit_message>
Add log4j implementation, written sample logs for login test.
</commit_message>
<xml_diff>
--- a/colombiasystemautomation/testdata/testdata.xlsx
+++ b/colombiasystemautomation/testdata/testdata.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Alerts" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="UserGroup" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="KnowledgeBase" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">HDPORTAL_EMAIL</t>
   </si>
@@ -35,58 +36,28 @@
     <t xml:space="preserve">MIA@27dec1</t>
   </si>
   <si>
-    <t xml:space="preserve">WEARER_NUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALERT_WEARER_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALERT_SEVERITY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALERT_START_DATE_FORMAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALERT_START_HOUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALERT_START_MINUTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALERT_NOTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSE_ALERT_NOTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacífica Rosalía Huerta, Automation-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manual alert is created...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closing alert...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Irfan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cc</t>
+    <t xml:space="preserve">USERGROUP_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UG_AUTOMATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNOWLEDGEBASE_ITEMNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNOWLEDGEBASE_SUBJECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNOWLEDGEBASE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KB_AUTOMATION_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the subject for knowledge base...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the description for knowledge base...</t>
   </si>
 </sst>
 </file>
@@ -274,7 +245,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -320,7 +291,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -328,85 +299,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.56"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>9010203040</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated log4 xml, updated knowledge base, alerts data in excel test data, updated test scripts of alerts and knowledgebase with data provider for get data, updated getcelldata method for accepting numeric values , updated config.properties for variable naming convention,CommonActions with log info, extent reports with log info, capturescreenshot method
</commit_message>
<xml_diff>
--- a/colombiasystemautomation/testdata/testdata.xlsx
+++ b/colombiasystemautomation/testdata/testdata.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="UserGroup" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="KnowledgeBase" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Alerts" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">HDPORTAL_EMAIL</t>
   </si>
@@ -58,14 +59,54 @@
   </si>
   <si>
     <t xml:space="preserve">This is the description for knowledge base...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERT_WEARER_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERT_SEVERITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERT_START_DATE_FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERT_START_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERT_START_MINUTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERT_NOTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEARER_NUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacífica Rosalía Huerta, Automation-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating manual alert….</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -149,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -163,6 +204,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,6 +349,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,15 +380,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,6 +412,87 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>9010203040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated scripts with excel data and log4j files and updated test data files for record credit data
</commit_message>
<xml_diff>
--- a/colombiasystemautomation/testdata/testdata.xlsx
+++ b/colombiasystemautomation/testdata/testdata.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="UserGroup" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="KnowledgeBase" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Alerts" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="RecordCreditNote" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">HDPORTAL_EMAIL</t>
   </si>
@@ -58,7 +59,7 @@
     <t xml:space="preserve">This is the subject for knowledge base...</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the description for knowledge base...</t>
+    <t xml:space="preserve">test</t>
   </si>
   <si>
     <t xml:space="preserve">ALERT_WEARER_NAME</t>
@@ -91,22 +92,56 @@
     <t xml:space="preserve">dd/MM/yyyy</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
     <t xml:space="preserve">40</t>
   </si>
   <si>
     <t xml:space="preserve">Creating manual alert….</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_UBIN_ITEMNUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_WEARER_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_NOTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_OBSERVATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_START_DATE_FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_END_DATE_FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wearer name from excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit notes from excel sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation from excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/10/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/10/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -211,7 +246,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,14 +333,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -313,7 +348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -346,18 +381,18 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -381,18 +416,18 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -403,7 +438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -432,24 +467,24 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -472,7 +507,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -482,16 +517,16 @@
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="1" t="n">
         <v>9010203040</v>
       </c>
     </row>
@@ -504,4 +539,77 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merging Record credit  note changes
</commit_message>
<xml_diff>
--- a/colombiasystemautomation/testdata/testdata.xlsx
+++ b/colombiasystemautomation/testdata/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -190,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,10 +208,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,13 +428,13 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
@@ -491,7 +487,7 @@
       <c r="F2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="1" t="n">
         <v>9010203040</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated test data for Recotrd credit note
</commit_message>
<xml_diff>
--- a/colombiasystemautomation/testdata/testdata.xlsx
+++ b/colombiasystemautomation/testdata/testdata.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="UserGroup" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="KnowledgeBase" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Alerts" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="RecordCreditNote" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">HDPORTAL_EMAIL</t>
   </si>
@@ -98,15 +99,52 @@
   </si>
   <si>
     <t xml:space="preserve">Creating manual alert….</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_UBIN_ITEMNUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_WEARER_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_NOTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_OBSERVATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_START_DATE_FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDCREDITNOTE_END_DATE_FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wearer name from excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit notes from excel sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation from excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/10/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/10/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -190,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +246,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,7 +418,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -500,4 +542,76 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.66"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated testng.xml file Updated Base Test class
</commit_message>
<xml_diff>
--- a/colombiasystemautomation/testdata/testdata.xlsx
+++ b/colombiasystemautomation/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="15585" windowHeight="150" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12825" windowHeight="6645" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Visits_CompletedVisits" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1:H20"/>
+  <oleSize ref="A1:F20"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -982,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1025,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>